<commit_message>
[refactor] Modify All files...
</commit_message>
<xml_diff>
--- a/additional/Reports/report.xlsx
+++ b/additional/Reports/report.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2122" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2119" uniqueCount="601">
   <si>
     <t>inventory_number</t>
   </si>
@@ -1538,9 +1538,6 @@
     <t>Кузьмин</t>
   </si>
   <si>
-    <t>Дустов</t>
-  </si>
-  <si>
     <t>Иван</t>
   </si>
   <si>
@@ -1658,9 +1655,6 @@
     <t>Владимир</t>
   </si>
   <si>
-    <t>Далерджон</t>
-  </si>
-  <si>
     <t>Иванович</t>
   </si>
   <si>
@@ -1784,9 +1778,6 @@
     <t>Дмитриевич</t>
   </si>
   <si>
-    <t>Юнусович</t>
-  </si>
-  <si>
     <t>Business Academy</t>
   </si>
   <si>
@@ -1814,25 +1805,22 @@
     <t>Office service</t>
   </si>
   <si>
+    <t>department__title</t>
+  </si>
+  <si>
+    <t>Human Resources Department</t>
+  </si>
+  <si>
+    <t>Technical department</t>
+  </si>
+  <si>
+    <t>Customer Service Department</t>
+  </si>
+  <si>
+    <t>Dep_Test_0001</t>
+  </si>
+  <si>
     <t>Div_Test_0001</t>
-  </si>
-  <si>
-    <t>department__title</t>
-  </si>
-  <si>
-    <t>Human Resources Department</t>
-  </si>
-  <si>
-    <t>Technical department</t>
-  </si>
-  <si>
-    <t>Customer Service Department</t>
-  </si>
-  <si>
-    <t>Dep_Test_0001</t>
-  </si>
-  <si>
-    <t>Dep_Test_4321</t>
   </si>
 </sst>
 </file>
@@ -2256,9 +2244,6 @@
       <c r="G2" t="s">
         <v>441</v>
       </c>
-      <c r="H2" t="s">
-        <v>439</v>
-      </c>
       <c r="I2" t="s">
         <v>452</v>
       </c>
@@ -9626,7 +9611,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D212"/>
+  <dimension ref="A1:D214"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -11958,15 +11943,40 @@
     </row>
     <row r="212" spans="1:4">
       <c r="A212">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B212">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C212" t="s">
         <v>439</v>
       </c>
       <c r="D212" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4">
+      <c r="A213">
+        <v>217</v>
+      </c>
+      <c r="B213">
+        <v>1</v>
+      </c>
+      <c r="C213" t="s">
+        <v>439</v>
+      </c>
+      <c r="D213" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4">
+      <c r="A214">
+        <v>217</v>
+      </c>
+      <c r="B214">
+        <v>42</v>
+      </c>
+      <c r="C214" t="s">
         <v>439</v>
       </c>
     </row>
@@ -11977,7 +11987,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -12008,16 +12018,16 @@
         <v>464</v>
       </c>
       <c r="B2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C2" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="F2">
         <v>3</v>
@@ -12028,16 +12038,16 @@
         <v>465</v>
       </c>
       <c r="B3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C3" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -12048,16 +12058,16 @@
         <v>466</v>
       </c>
       <c r="B4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C4" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -12068,16 +12078,16 @@
         <v>467</v>
       </c>
       <c r="B5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C5" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -12088,16 +12098,16 @@
         <v>468</v>
       </c>
       <c r="B6" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C6" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -12108,16 +12118,16 @@
         <v>469</v>
       </c>
       <c r="B7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -12128,16 +12138,16 @@
         <v>470</v>
       </c>
       <c r="B8" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="D8">
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="F8">
         <v>3</v>
@@ -12148,16 +12158,16 @@
         <v>471</v>
       </c>
       <c r="B9" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C9" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="F9">
         <v>3</v>
@@ -12168,16 +12178,16 @@
         <v>472</v>
       </c>
       <c r="B10" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C10" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D10">
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="F10">
         <v>3</v>
@@ -12188,16 +12198,16 @@
         <v>473</v>
       </c>
       <c r="B11" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C11" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="F11">
         <v>3</v>
@@ -12208,16 +12218,16 @@
         <v>474</v>
       </c>
       <c r="B12" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C12" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="F12">
         <v>3</v>
@@ -12228,16 +12238,16 @@
         <v>475</v>
       </c>
       <c r="B13" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C13" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="F13">
         <v>3</v>
@@ -12248,16 +12258,16 @@
         <v>476</v>
       </c>
       <c r="B14" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C14" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="D14">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -12268,16 +12278,16 @@
         <v>477</v>
       </c>
       <c r="B15" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C15" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D15">
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="F15">
         <v>3</v>
@@ -12288,16 +12298,16 @@
         <v>478</v>
       </c>
       <c r="B16" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C16" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D16">
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="F16">
         <v>3</v>
@@ -12308,16 +12318,16 @@
         <v>479</v>
       </c>
       <c r="B17" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C17" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="F17">
         <v>9</v>
@@ -12328,16 +12338,16 @@
         <v>480</v>
       </c>
       <c r="B18" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C18" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="F18">
         <v>9</v>
@@ -12348,16 +12358,16 @@
         <v>481</v>
       </c>
       <c r="B19" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C19" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="F19">
         <v>9</v>
@@ -12368,16 +12378,16 @@
         <v>482</v>
       </c>
       <c r="B20" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C20" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D20">
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="F20">
         <v>9</v>
@@ -12388,16 +12398,16 @@
         <v>483</v>
       </c>
       <c r="B21" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C21" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="F21">
         <v>9</v>
@@ -12408,16 +12418,16 @@
         <v>484</v>
       </c>
       <c r="B22" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C22" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D22">
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="F22">
         <v>9</v>
@@ -12428,16 +12438,16 @@
         <v>485</v>
       </c>
       <c r="B23" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C23" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D23">
         <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="F23">
         <v>9</v>
@@ -12448,16 +12458,16 @@
         <v>486</v>
       </c>
       <c r="B24" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C24" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="D24">
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="F24">
         <v>9</v>
@@ -12468,16 +12478,16 @@
         <v>487</v>
       </c>
       <c r="B25" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C25" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D25">
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="F25">
         <v>9</v>
@@ -12488,16 +12498,16 @@
         <v>488</v>
       </c>
       <c r="B26" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C26" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="F26">
         <v>8</v>
@@ -12508,16 +12518,16 @@
         <v>489</v>
       </c>
       <c r="B27" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C27" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="F27">
         <v>8</v>
@@ -12528,16 +12538,16 @@
         <v>490</v>
       </c>
       <c r="B28" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C28" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="F28">
         <v>8</v>
@@ -12548,16 +12558,16 @@
         <v>491</v>
       </c>
       <c r="B29" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C29" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="F29">
         <v>8</v>
@@ -12568,16 +12578,16 @@
         <v>492</v>
       </c>
       <c r="B30" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C30" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="D30">
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="F30">
         <v>8</v>
@@ -12588,16 +12598,16 @@
         <v>493</v>
       </c>
       <c r="B31" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C31" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="D31">
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="F31">
         <v>8</v>
@@ -12608,16 +12618,16 @@
         <v>494</v>
       </c>
       <c r="B32" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C32" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D32">
         <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="F32">
         <v>8</v>
@@ -12628,16 +12638,16 @@
         <v>495</v>
       </c>
       <c r="B33" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C33" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D33">
         <v>3</v>
       </c>
       <c r="E33" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="F33">
         <v>8</v>
@@ -12648,16 +12658,16 @@
         <v>496</v>
       </c>
       <c r="B34" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C34" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D34">
         <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="F34">
         <v>8</v>
@@ -12668,16 +12678,16 @@
         <v>497</v>
       </c>
       <c r="B35" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C35" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="F35">
         <v>5</v>
@@ -12688,16 +12698,16 @@
         <v>498</v>
       </c>
       <c r="B36" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C36" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="F36">
         <v>6</v>
@@ -12708,16 +12718,16 @@
         <v>499</v>
       </c>
       <c r="B37" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C37" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="F37">
         <v>7</v>
@@ -12728,16 +12738,16 @@
         <v>500</v>
       </c>
       <c r="B38" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C38" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="D38">
         <v>2</v>
       </c>
       <c r="E38" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="F38">
         <v>5</v>
@@ -12748,16 +12758,16 @@
         <v>501</v>
       </c>
       <c r="B39" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C39" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D39">
         <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="F39">
         <v>6</v>
@@ -12768,16 +12778,16 @@
         <v>502</v>
       </c>
       <c r="B40" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C40" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="D40">
         <v>2</v>
       </c>
       <c r="E40" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="F40">
         <v>7</v>
@@ -12788,16 +12798,16 @@
         <v>503</v>
       </c>
       <c r="B41" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C41" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="D41">
         <v>3</v>
       </c>
       <c r="E41" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="F41">
         <v>5</v>
@@ -12808,16 +12818,16 @@
         <v>504</v>
       </c>
       <c r="B42" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C42" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D42">
         <v>3</v>
       </c>
       <c r="E42" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="F42">
         <v>6</v>
@@ -12828,38 +12838,18 @@
         <v>505</v>
       </c>
       <c r="B43" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C43" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D43">
         <v>3</v>
       </c>
       <c r="E43" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="F43">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" t="s">
-        <v>506</v>
-      </c>
-      <c r="B44" t="s">
-        <v>546</v>
-      </c>
-      <c r="C44" t="s">
-        <v>588</v>
-      </c>
-      <c r="D44">
-        <v>15</v>
-      </c>
-      <c r="E44" t="s">
-        <v>598</v>
-      </c>
-      <c r="F44">
         <v>7</v>
       </c>
     </row>
@@ -12878,7 +12868,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -12886,82 +12876,82 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="B2" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="B3" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="B4" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="B5" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="B6" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="B7" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="B8" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="B9" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="B10" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="B11" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
   </sheetData>
@@ -12971,7 +12961,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -12984,27 +12974,22 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>